<commit_message>
EPBDS-13605 Performance Improvement: The expression in the return cell is executed, despite the fact that corresponded the rule was not matched.
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9096-ConditionExpressionInvocationTest.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9096-ConditionExpressionInvocationTest.xlsx
@@ -1,30 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpikus\.openl-webstudio\user-workspace\admin\EPBDS-9096\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\openl-tablets\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF19322A-6651-43AF-B373-E72D7F295824}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9178A6E8-CC0D-4299-B8C6-70ACECFDD2C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6860" yWindow="3410" windowWidth="21960" windowHeight="14870" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Preconditions" sheetId="3" r:id="rId1"/>
     <sheet name="Testing" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -656,22 +648,22 @@
       <selection activeCell="C11" sqref="C11:E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>10</v>
       </c>
@@ -682,7 +674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -693,7 +685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -704,14 +696,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
@@ -725,7 +717,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>2</v>
       </c>
@@ -739,7 +731,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>3</v>
       </c>
@@ -753,7 +745,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>4</v>
       </c>
@@ -767,18 +759,18 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
       <c r="E14" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>20</v>
       </c>
@@ -786,7 +778,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>22</v>
       </c>
@@ -794,7 +786,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>23</v>
       </c>
@@ -802,13 +794,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B25" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>20</v>
       </c>
@@ -816,7 +808,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>22</v>
       </c>
@@ -824,7 +816,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>23</v>
       </c>
@@ -832,16 +824,16 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C29" s="2"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B32" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>20</v>
       </c>
@@ -849,7 +841,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>22</v>
       </c>
@@ -857,7 +849,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>23</v>
       </c>
@@ -882,20 +874,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:H168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="C139" sqref="C139"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="39.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.08984375" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
         <v>46</v>
       </c>
@@ -903,7 +895,7 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>16</v>
       </c>
@@ -917,7 +909,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>8</v>
       </c>
@@ -931,7 +923,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>8</v>
       </c>
@@ -945,7 +937,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B7">
         <v>8</v>
       </c>
@@ -959,7 +951,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>7</v>
       </c>
@@ -973,7 +965,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B9">
         <v>7</v>
       </c>
@@ -987,7 +979,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>7</v>
       </c>
@@ -1001,7 +993,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B11">
         <v>10</v>
       </c>
@@ -1015,7 +1007,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>10</v>
       </c>
@@ -1029,7 +1021,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B13">
         <v>10</v>
       </c>
@@ -1043,7 +1035,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B14">
         <v>12</v>
       </c>
@@ -1057,7 +1049,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B15">
         <v>12</v>
       </c>
@@ -1071,7 +1063,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>12</v>
       </c>
@@ -1085,7 +1077,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B17">
         <v>8</v>
       </c>
@@ -1099,7 +1091,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B18">
         <v>8</v>
       </c>
@@ -1113,7 +1105,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B19">
         <v>8</v>
       </c>
@@ -1127,21 +1119,21 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
       <c r="E20" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C21" s="2"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B23" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>20</v>
       </c>
@@ -1149,7 +1141,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>26</v>
       </c>
@@ -1157,7 +1149,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>5</v>
       </c>
@@ -1165,7 +1157,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B30" s="3" t="s">
         <v>27</v>
       </c>
@@ -1176,7 +1168,7 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>28</v>
       </c>
@@ -1196,7 +1188,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>49</v>
       </c>
@@ -1219,7 +1211,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>50</v>
       </c>
@@ -1242,7 +1234,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>29</v>
       </c>
@@ -1265,7 +1257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>51</v>
       </c>
@@ -1288,7 +1280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>52</v>
       </c>
@@ -1296,22 +1288,22 @@
         <v>52</v>
       </c>
       <c r="D36">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E36">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F36">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G36">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>30</v>
       </c>
@@ -1334,7 +1326,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B43" s="3" t="s">
         <v>54</v>
       </c>
@@ -1342,7 +1334,7 @@
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>6</v>
       </c>
@@ -1356,7 +1348,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>17</v>
       </c>
@@ -1367,7 +1359,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>18</v>
       </c>
@@ -1381,7 +1373,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>16</v>
       </c>
@@ -1395,7 +1387,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B48">
         <v>8</v>
       </c>
@@ -1409,7 +1401,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B49">
         <v>8</v>
       </c>
@@ -1423,7 +1415,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B50">
         <v>8</v>
       </c>
@@ -1437,7 +1429,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B51">
         <v>7</v>
       </c>
@@ -1451,7 +1443,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B52">
         <v>7</v>
       </c>
@@ -1465,7 +1457,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B53">
         <v>7</v>
       </c>
@@ -1479,7 +1471,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B54">
         <v>10</v>
       </c>
@@ -1493,7 +1485,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B55">
         <v>10</v>
       </c>
@@ -1507,7 +1499,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B56">
         <v>10</v>
       </c>
@@ -1521,7 +1513,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B57">
         <v>12</v>
       </c>
@@ -1535,7 +1527,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B58">
         <v>12</v>
       </c>
@@ -1549,7 +1541,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B59">
         <v>12</v>
       </c>
@@ -1563,7 +1555,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B60">
         <v>8</v>
       </c>
@@ -1577,7 +1569,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B61">
         <v>8</v>
       </c>
@@ -1591,7 +1583,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B62">
         <v>8</v>
       </c>
@@ -1605,18 +1597,18 @@
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.35">
       <c r="E63" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B66" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C66" s="3"/>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
         <v>20</v>
       </c>
@@ -1624,7 +1616,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B68" t="s">
         <v>26</v>
       </c>
@@ -1632,7 +1624,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B69" t="s">
         <v>5</v>
       </c>
@@ -1640,7 +1632,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B75" s="3" t="s">
         <v>32</v>
       </c>
@@ -1651,7 +1643,7 @@
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B76" t="s">
         <v>28</v>
       </c>
@@ -1671,7 +1663,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B77" t="s">
         <v>49</v>
       </c>
@@ -1694,7 +1686,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B78" t="s">
         <v>50</v>
       </c>
@@ -1717,7 +1709,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B79" t="s">
         <v>29</v>
       </c>
@@ -1740,7 +1732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B80" t="s">
         <v>51</v>
       </c>
@@ -1763,7 +1755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
         <v>52</v>
       </c>
@@ -1771,22 +1763,22 @@
         <v>52</v>
       </c>
       <c r="D81">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E81">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F81">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G81">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H81">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B82" t="s">
         <v>30</v>
       </c>
@@ -1809,7 +1801,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B89" s="3" t="s">
         <v>57</v>
       </c>
@@ -1817,7 +1809,7 @@
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
     </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B90" t="s">
         <v>16</v>
       </c>
@@ -1831,7 +1823,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B91">
         <v>8</v>
       </c>
@@ -1845,7 +1837,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B92" s="2" t="s">
         <v>60</v>
       </c>
@@ -1859,7 +1851,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B93">
         <v>8</v>
       </c>
@@ -1873,7 +1865,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B94">
         <v>7</v>
       </c>
@@ -1887,7 +1879,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B95" s="2" t="s">
         <v>59</v>
       </c>
@@ -1901,7 +1893,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B96">
         <v>7</v>
       </c>
@@ -1915,7 +1907,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B97">
         <v>10</v>
       </c>
@@ -1929,7 +1921,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B98" s="2" t="s">
         <v>58</v>
       </c>
@@ -1943,7 +1935,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B99">
         <v>10</v>
       </c>
@@ -1957,7 +1949,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B100">
         <v>12</v>
       </c>
@@ -1971,7 +1963,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B101">
         <v>12</v>
       </c>
@@ -1985,7 +1977,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B102">
         <v>12</v>
       </c>
@@ -1999,7 +1991,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B103">
         <v>8</v>
       </c>
@@ -2013,7 +2005,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="104" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B104">
         <v>8</v>
       </c>
@@ -2027,7 +2019,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="105" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B105">
         <v>8</v>
       </c>
@@ -2041,21 +2033,21 @@
         <v>53</v>
       </c>
     </row>
-    <row r="106" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:5" x14ac:dyDescent="0.35">
       <c r="E106" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="107" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C107" s="2"/>
     </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B109" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C109" s="3"/>
     </row>
-    <row r="110" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B110" t="s">
         <v>20</v>
       </c>
@@ -2063,7 +2055,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="111" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B111" t="s">
         <v>26</v>
       </c>
@@ -2071,7 +2063,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="112" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B112" t="s">
         <v>5</v>
       </c>
@@ -2079,7 +2071,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="116" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B116" s="3" t="s">
         <v>65</v>
       </c>
@@ -2090,7 +2082,7 @@
       <c r="G116" s="3"/>
       <c r="H116" s="3"/>
     </row>
-    <row r="117" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B117" t="s">
         <v>28</v>
       </c>
@@ -2110,7 +2102,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B118" t="s">
         <v>49</v>
       </c>
@@ -2133,7 +2125,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="119" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B119" t="s">
         <v>50</v>
       </c>
@@ -2156,7 +2148,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="120" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B120" t="s">
         <v>29</v>
       </c>
@@ -2179,7 +2171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B121" t="s">
         <v>51</v>
       </c>
@@ -2202,7 +2194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B122" t="s">
         <v>52</v>
       </c>
@@ -2210,22 +2202,22 @@
         <v>52</v>
       </c>
       <c r="D122">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E122">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F122">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G122">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H122">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="123" spans="2:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B123" t="s">
         <v>30</v>
       </c>
@@ -2248,7 +2240,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="129" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B129" s="3" t="s">
         <v>66</v>
       </c>
@@ -2256,7 +2248,7 @@
       <c r="D129" s="3"/>
       <c r="E129" s="3"/>
     </row>
-    <row r="130" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B130" t="s">
         <v>6</v>
       </c>
@@ -2270,7 +2262,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="131" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B131" t="s">
         <v>17</v>
       </c>
@@ -2281,7 +2273,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="132" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B132" t="s">
         <v>18</v>
       </c>
@@ -2295,7 +2287,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="133" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B133" t="s">
         <v>16</v>
       </c>
@@ -2309,7 +2301,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="134" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B134">
         <v>8</v>
       </c>
@@ -2323,7 +2315,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="135" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B135" s="2" t="s">
         <v>60</v>
       </c>
@@ -2337,7 +2329,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="136" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B136">
         <v>8</v>
       </c>
@@ -2351,7 +2343,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B137">
         <v>7</v>
       </c>
@@ -2365,7 +2357,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="138" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B138" s="2" t="s">
         <v>59</v>
       </c>
@@ -2379,7 +2371,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="139" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B139">
         <v>7</v>
       </c>
@@ -2393,7 +2385,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="140" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B140">
         <v>10</v>
       </c>
@@ -2407,7 +2399,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="141" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B141" s="2" t="s">
         <v>58</v>
       </c>
@@ -2421,7 +2413,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="142" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B142">
         <v>10</v>
       </c>
@@ -2435,7 +2427,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="143" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B143">
         <v>12</v>
       </c>
@@ -2449,7 +2441,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="144" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B144">
         <v>12</v>
       </c>
@@ -2463,7 +2455,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="145" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B145">
         <v>12</v>
       </c>
@@ -2477,7 +2469,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="146" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B146">
         <v>8</v>
       </c>
@@ -2491,7 +2483,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="147" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B147">
         <v>8</v>
       </c>
@@ -2505,7 +2497,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="148" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B148">
         <v>8</v>
       </c>
@@ -2519,18 +2511,18 @@
         <v>53</v>
       </c>
     </row>
-    <row r="149" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:5" x14ac:dyDescent="0.35">
       <c r="E149" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="152" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B152" s="3" t="s">
         <v>67</v>
       </c>
       <c r="C152" s="3"/>
     </row>
-    <row r="153" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B153" t="s">
         <v>20</v>
       </c>
@@ -2538,7 +2530,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="154" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B154" t="s">
         <v>26</v>
       </c>
@@ -2546,7 +2538,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="155" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B155" t="s">
         <v>5</v>
       </c>
@@ -2554,7 +2546,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="161" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B161" s="3" t="s">
         <v>68</v>
       </c>
@@ -2565,7 +2557,7 @@
       <c r="G161" s="3"/>
       <c r="H161" s="3"/>
     </row>
-    <row r="162" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B162" t="s">
         <v>28</v>
       </c>
@@ -2585,7 +2577,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="163" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B163" t="s">
         <v>49</v>
       </c>
@@ -2608,7 +2600,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="164" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B164" t="s">
         <v>50</v>
       </c>
@@ -2631,7 +2623,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="165" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B165" t="s">
         <v>29</v>
       </c>
@@ -2654,7 +2646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B166" t="s">
         <v>51</v>
       </c>
@@ -2677,7 +2669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B167" t="s">
         <v>52</v>
       </c>
@@ -2685,22 +2677,22 @@
         <v>52</v>
       </c>
       <c r="D167">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E167">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F167">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G167">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H167">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="168" spans="2:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B168" t="s">
         <v>30</v>
       </c>
@@ -2725,8 +2717,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B129:E129"/>
-    <mergeCell ref="B152:C152"/>
     <mergeCell ref="B161:H161"/>
     <mergeCell ref="B66:C66"/>
     <mergeCell ref="B30:H30"/>
@@ -2737,6 +2727,8 @@
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B43:E43"/>
     <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B129:E129"/>
+    <mergeCell ref="B152:C152"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>